<commit_message>
added loading of xlsx file
</commit_message>
<xml_diff>
--- a/src/main/resources/pp_structure.xlsx
+++ b/src/main/resources/pp_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">Veta</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Nazov premennej</t>
   </si>
   <si>
+    <t xml:space="preserve">Format</t>
+  </si>
+  <si>
     <t xml:space="preserve">kód úvodnej vety</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">fileCreated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ddmmrrrr</t>
   </si>
   <si>
     <t xml:space="preserve">poradové číslo súboru v rámci 12 mesiacov</t>
@@ -190,7 +196,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,18 +281,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.95"/>
   </cols>
   <sheetData>
@@ -306,6 +312,9 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -315,13 +324,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,13 +341,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>34</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,13 +358,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>34</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,13 +375,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,13 +395,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,13 +412,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,13 +429,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,13 +446,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,13 +463,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added generators for model classes
</commit_message>
<xml_diff>
--- a/src/main/resources/pp_structure.xlsx
+++ b/src/main/resources/pp_structure.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PPE" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ppe" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="pod" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t xml:space="preserve">Veta</t>
   </si>
@@ -95,6 +96,156 @@
   </si>
   <si>
     <t xml:space="preserve">payOutDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kód dátovej vety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meno a priezvisko adresáta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recipientFullName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ďalší identifikačný údaj adresáta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recipientOtherIdentifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ulica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">číslo domu (orientačné číslo) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">municipality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poštové smerovacie číslo dodávacej pošty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postOfficePostalCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adresa – poznámka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressNote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suma (9999999.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cena (9999.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kód služby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serviceCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kód adresáta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recipientCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">účel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kontaktný e-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telefón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kód koncovej vety </t>
+  </si>
+  <si>
+    <t xml:space="preserve">počet poukazov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voucherCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suma celkom (9999999999.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ceny celkom (9999999.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celková úhrnná suma (9999999999.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">číslo okresnej pečiatky určeného pracoviska SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stampNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deň prijatia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dayReceived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mesiac prijatia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthReceived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rok prijatia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yearReceived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">podacie číslo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suma (9999999.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cena (9999.9)</t>
   </si>
 </sst>
 </file>
@@ -196,11 +347,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,22 +432,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -329,7 +481,7 @@
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -473,6 +625,361 @@
       </c>
       <c r="F10" s="0" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>9999999.99</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>9999.99</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <v>9999999999.99</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <v>9999999.99</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="4" t="n">
+        <v>9999999999.99</v>
       </c>
     </row>
   </sheetData>
@@ -484,4 +991,357 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>9999999999.99</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>9999999.99</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>9999999999.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>